<commit_message>
Renamed all attributes to understandable names
</commit_message>
<xml_diff>
--- a/dataset/Attributsuebersicht.xlsx
+++ b/dataset/Attributsuebersicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Repositories\himalayaClassificationProject\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E77F8D9-F36E-4F99-BBE4-A8E0C3E87CE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84A0577-6B28-4770-B31E-7D679A51C54B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15630" yWindow="6210" windowWidth="19200" windowHeight="5380" xr2:uid="{62A842C3-D8EC-4167-AF7B-9277287D47E0}"/>
+    <workbookView visibility="hidden" xWindow="15630" yWindow="6210" windowWidth="19200" windowHeight="5380" xr2:uid="{62A842C3-D8EC-4167-AF7B-9277287D47E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2776CCE6-3D3E-4536-8892-F21382FCC929}">
   <dimension ref="B1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">

</xml_diff>